<commit_message>
Set up test optimization for ply orientation
</commit_message>
<xml_diff>
--- a/MATLAB/Structures/HW5_P1_OutputResults.xlsx
+++ b/MATLAB/Structures/HW5_P1_OutputResults.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
   <si>
     <t>Layup ID:</t>
   </si>
@@ -730,7 +730,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="135">
+  <borders count="193">
     <border>
       <left/>
       <right/>
@@ -1004,11 +1004,69 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -1254,6 +1312,64 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="132" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="133" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="137" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="138" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="139" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="143" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="144" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="145" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="146" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="147" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="148" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="149" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="150" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="159" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="160" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="166" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="167" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="170" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="171" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="173" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="174" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="180" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="181" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="184" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="185" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="186" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="187" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="188" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="189" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="190" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="191" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="192" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2100,7 +2216,7 @@
       </c>
       <c r="F46" s="40"/>
       <c r="G46" s="40"/>
-      <c r="H46" s="175" t="s">
+      <c r="H46" s="233" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2113,12 +2229,12 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="171" t="s">
+      <c r="E47" s="229" t="s">
         <v>65</v>
       </c>
       <c r="F47" s="40"/>
       <c r="G47" s="40"/>
-      <c r="H47" s="175" t="s">
+      <c r="H47" s="233" t="s">
         <v>67</v>
       </c>
       <c r="I47" s="3"/>

</xml_diff>